<commit_message>
Signed-off-by: Shuiqing He <sqhe@cs.hku.hk>
</commit_message>
<xml_diff>
--- a/temp/bill.xlsx
+++ b/temp/bill.xlsx
@@ -62,7 +62,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -357,7 +357,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -423,8 +423,7 @@
         <v>110</v>
       </c>
       <c r="H5">
-        <f>SUM(H1:H4)</f>
-        <v>134</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -433,6 +432,10 @@
       </c>
       <c r="C6">
         <v>598</v>
+      </c>
+      <c r="H6">
+        <f>SUM(H1:H5)</f>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:10">

</xml_diff>